<commit_message>
address getUsername bug, making map visible on small screens (mobile), and added disclaimer for user safety when traveling to sites.
</commit_message>
<xml_diff>
--- a/resources/PA Historical Finder Risks Analysis.xlsx
+++ b/resources/PA Historical Finder Risks Analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shannon/Documents/Software Engineering and Sys Analys Principles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shannon/Documents/GitHub/CISC397/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Asset</t>
   </si>
@@ -108,6 +108,21 @@
   </si>
   <si>
     <t>Have a script that, when ran, will repopulate data store with records stored on a plain text file.</t>
+  </si>
+  <si>
+    <t>System not having protection from spam bots</t>
+  </si>
+  <si>
+    <t>Email address being subject to spam and virsuses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bots sending spam email to users or scraping system user web interface for emails. </t>
+  </si>
+  <si>
+    <t>Not having a spam bot detection mechanism</t>
+  </si>
+  <si>
+    <t>Having a Captcha upon login.</t>
   </si>
 </sst>
 </file>
@@ -194,9 +209,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -207,6 +219,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,7 +540,7 @@
   <dimension ref="A3:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,7 +577,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="6" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -583,7 +598,7 @@
     </row>
     <row r="5" spans="1:7" s="9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -602,26 +617,45 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:7" s="11" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="7" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
-      <c r="B7" s="13"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="12"/>
     </row>
     <row r="9" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="12"/>
     </row>
     <row r="10" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="12"/>
     </row>
     <row r="11" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="12"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -665,8 +699,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="10" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="10" t="s">

</xml_diff>